<commit_message>
Import del excel. Si hay un usuario que no existe, no se va a insertar el post
</commit_message>
<xml_diff>
--- a/posts10102018.xlsx
+++ b/posts10102018.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>AUTHOR</t>
   </si>
@@ -35,29 +35,65 @@
     <t>TEXT</t>
   </si>
   <si>
-    <t>DATE CREATE</t>
-  </si>
-  <si>
-    <t>Eva</t>
-  </si>
-  <si>
     <t>Prueba importación</t>
   </si>
   <si>
     <t>esta es una prueba con tildes</t>
+  </si>
+  <si>
+    <t>ACTIVE</t>
+  </si>
+  <si>
+    <t>Prueba importación 2</t>
+  </si>
+  <si>
+    <t>Prueba importacion 3</t>
+  </si>
+  <si>
+    <t>Aquí no tenemos texto</t>
+  </si>
+  <si>
+    <t>Vamos a ir a la playa</t>
+  </si>
+  <si>
+    <t>evau</t>
+  </si>
+  <si>
+    <t>Carla</t>
+  </si>
+  <si>
+    <t>No va</t>
+  </si>
+  <si>
+    <t>hdsh</t>
+  </si>
+  <si>
+    <t>sjaimesm</t>
+  </si>
+  <si>
+    <t>Hola</t>
+  </si>
+  <si>
+    <t>hola</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,9 +116,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -363,15 +400,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
@@ -388,24 +424,81 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1">
-        <v>43383</v>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>